<commit_message>
chronicled loading, cleaning, and transforming/ merging data sets
</commit_message>
<xml_diff>
--- a/Data set C.xlsx
+++ b/Data set C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\2025-CAH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619722BB-D1F9-40C7-8C5A-16B69001886B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4704C10E-B5D1-46A1-AB59-19C6459F1909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{50EF7171-71BD-4C55-BA0F-C7AFC7B5920C}"/>
   </bookViews>
@@ -26,8 +26,8 @@
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="21" r:id="rId5"/>
-    <pivotCache cacheId="22" r:id="rId6"/>
-    <pivotCache cacheId="24" r:id="rId7"/>
+    <pivotCache cacheId="25" r:id="rId6"/>
+    <pivotCache cacheId="26" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4063" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4072" uniqueCount="19">
   <si>
     <t xml:space="preserve">identifier </t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Dataset B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min of identifier </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max of identifier </t>
   </si>
 </sst>
 </file>
@@ -239,7 +245,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,6 +425,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -580,7 +592,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -590,6 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -15533,8 +15546,50 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3D130CCA-38D7-4DE4-88FD-53A42B07AA23}" name="PivotTable8" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="G14:K23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C9ECD36-244A-4894-B5EA-49F08E8FE456}" name="PivotTable19" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A7:A8" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="3">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Max of identifier " fld="0" subtotal="max" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3D130CCA-38D7-4DE4-88FD-53A42B07AA23}" name="PivotTable8" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I18:M27" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
@@ -15623,9 +15678,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{35F2D6FF-FEE3-438E-94D0-636C6E9B31F6}" name="PivotTable6" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="G2:J7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{35F2D6FF-FEE3-438E-94D0-636C6E9B31F6}" name="PivotTable6" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I2:L7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
@@ -15690,9 +15745,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{44DF8454-BF05-480A-8469-29E5F0A53154}" name="PivotTable3" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A2:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{44DF8454-BF05-480A-8469-29E5F0A53154}" name="PivotTable3" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="C2:D6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
@@ -15746,9 +15801,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3FD308F1-1BEA-43C5-8FEE-A7B770B702E6}" name="PivotTable5" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A14:E19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3FD308F1-1BEA-43C5-8FEE-A7B770B702E6}" name="PivotTable5" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="C18:G23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
@@ -15818,9 +15873,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CC7FE067-390E-4ADA-B753-005D4D59B495}" name="PivotTable4" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A9:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="C10:D13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" showAll="0">
       <items count="753">
@@ -16619,6 +16674,2592 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{63B7685D-6994-4358-AB28-D7C1A73D14F3}" name="PivotTable18" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A5:A6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="3">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Min of identifier " fld="0" subtotal="min" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F6E7E337-DB19-4A7A-8F02-A0C6FA6C213E}" name="PivotTable17" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A15:A16" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" showAll="0">
+      <items count="753">
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="207"/>
+        <item x="208"/>
+        <item x="209"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="210"/>
+        <item x="211"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="212"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="213"/>
+        <item x="33"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="182"/>
+        <item x="34"/>
+        <item x="214"/>
+        <item x="35"/>
+        <item x="183"/>
+        <item x="184"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="36"/>
+        <item x="185"/>
+        <item x="215"/>
+        <item x="186"/>
+        <item x="187"/>
+        <item x="37"/>
+        <item x="216"/>
+        <item x="188"/>
+        <item x="189"/>
+        <item x="217"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="190"/>
+        <item x="218"/>
+        <item x="191"/>
+        <item x="219"/>
+        <item x="40"/>
+        <item x="220"/>
+        <item x="41"/>
+        <item x="221"/>
+        <item x="6"/>
+        <item x="42"/>
+        <item x="192"/>
+        <item x="193"/>
+        <item x="43"/>
+        <item x="222"/>
+        <item x="44"/>
+        <item x="7"/>
+        <item x="194"/>
+        <item x="45"/>
+        <item x="8"/>
+        <item x="223"/>
+        <item x="224"/>
+        <item x="46"/>
+        <item x="225"/>
+        <item x="47"/>
+        <item x="195"/>
+        <item x="226"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="227"/>
+        <item x="228"/>
+        <item x="229"/>
+        <item x="230"/>
+        <item x="9"/>
+        <item x="50"/>
+        <item x="196"/>
+        <item x="197"/>
+        <item x="231"/>
+        <item x="232"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="198"/>
+        <item x="233"/>
+        <item x="199"/>
+        <item x="234"/>
+        <item x="200"/>
+        <item x="69"/>
+        <item x="235"/>
+        <item x="201"/>
+        <item x="10"/>
+        <item x="70"/>
+        <item x="11"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="202"/>
+        <item x="249"/>
+        <item x="250"/>
+        <item x="251"/>
+        <item x="203"/>
+        <item x="204"/>
+        <item x="73"/>
+        <item x="12"/>
+        <item x="252"/>
+        <item x="13"/>
+        <item x="74"/>
+        <item x="253"/>
+        <item x="205"/>
+        <item x="75"/>
+        <item x="14"/>
+        <item x="206"/>
+        <item x="236"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="51"/>
+        <item x="254"/>
+        <item x="78"/>
+        <item x="52"/>
+        <item x="79"/>
+        <item x="53"/>
+        <item x="237"/>
+        <item x="80"/>
+        <item x="54"/>
+        <item x="81"/>
+        <item x="255"/>
+        <item x="256"/>
+        <item x="257"/>
+        <item x="238"/>
+        <item x="258"/>
+        <item x="82"/>
+        <item x="239"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="259"/>
+        <item x="240"/>
+        <item x="241"/>
+        <item x="83"/>
+        <item x="260"/>
+        <item x="242"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="243"/>
+        <item x="57"/>
+        <item x="86"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="244"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="89"/>
+        <item x="261"/>
+        <item x="90"/>
+        <item x="62"/>
+        <item x="262"/>
+        <item x="63"/>
+        <item x="245"/>
+        <item x="246"/>
+        <item x="64"/>
+        <item x="91"/>
+        <item x="263"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="92"/>
+        <item x="93"/>
+        <item x="247"/>
+        <item x="264"/>
+        <item x="265"/>
+        <item x="97"/>
+        <item x="266"/>
+        <item x="248"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item x="100"/>
+        <item x="284"/>
+        <item x="101"/>
+        <item x="102"/>
+        <item x="285"/>
+        <item x="94"/>
+        <item x="286"/>
+        <item x="287"/>
+        <item x="288"/>
+        <item x="267"/>
+        <item x="268"/>
+        <item x="289"/>
+        <item x="103"/>
+        <item x="269"/>
+        <item x="104"/>
+        <item x="270"/>
+        <item x="95"/>
+        <item x="271"/>
+        <item x="272"/>
+        <item x="96"/>
+        <item x="273"/>
+        <item x="105"/>
+        <item x="274"/>
+        <item x="290"/>
+        <item x="106"/>
+        <item x="291"/>
+        <item x="275"/>
+        <item x="292"/>
+        <item x="107"/>
+        <item x="108"/>
+        <item x="276"/>
+        <item x="277"/>
+        <item x="293"/>
+        <item x="278"/>
+        <item x="279"/>
+        <item x="280"/>
+        <item x="294"/>
+        <item x="300"/>
+        <item x="281"/>
+        <item x="117"/>
+        <item x="118"/>
+        <item x="282"/>
+        <item x="301"/>
+        <item x="283"/>
+        <item x="302"/>
+        <item x="119"/>
+        <item x="295"/>
+        <item x="120"/>
+        <item x="303"/>
+        <item x="296"/>
+        <item x="297"/>
+        <item x="109"/>
+        <item x="298"/>
+        <item x="304"/>
+        <item x="305"/>
+        <item x="110"/>
+        <item x="299"/>
+        <item x="306"/>
+        <item x="124"/>
+        <item x="125"/>
+        <item x="310"/>
+        <item x="111"/>
+        <item x="126"/>
+        <item x="127"/>
+        <item x="112"/>
+        <item x="136"/>
+        <item x="113"/>
+        <item x="114"/>
+        <item x="115"/>
+        <item x="116"/>
+        <item x="307"/>
+        <item x="131"/>
+        <item x="308"/>
+        <item x="121"/>
+        <item x="132"/>
+        <item x="311"/>
+        <item x="133"/>
+        <item x="122"/>
+        <item x="137"/>
+        <item x="138"/>
+        <item x="367"/>
+        <item x="312"/>
+        <item x="123"/>
+        <item x="317"/>
+        <item x="318"/>
+        <item x="309"/>
+        <item x="313"/>
+        <item x="128"/>
+        <item x="319"/>
+        <item x="314"/>
+        <item x="129"/>
+        <item x="315"/>
+        <item x="130"/>
+        <item x="320"/>
+        <item x="316"/>
+        <item x="141"/>
+        <item x="142"/>
+        <item x="145"/>
+        <item x="134"/>
+        <item x="146"/>
+        <item x="321"/>
+        <item x="325"/>
+        <item x="322"/>
+        <item x="323"/>
+        <item x="135"/>
+        <item x="326"/>
+        <item x="327"/>
+        <item x="368"/>
+        <item x="139"/>
+        <item x="140"/>
+        <item x="157"/>
+        <item x="158"/>
+        <item x="324"/>
+        <item x="159"/>
+        <item x="328"/>
+        <item x="329"/>
+        <item x="160"/>
+        <item x="369"/>
+        <item x="161"/>
+        <item x="162"/>
+        <item x="143"/>
+        <item x="144"/>
+        <item x="330"/>
+        <item x="350"/>
+        <item x="351"/>
+        <item x="370"/>
+        <item x="163"/>
+        <item x="352"/>
+        <item x="164"/>
+        <item x="331"/>
+        <item x="353"/>
+        <item x="165"/>
+        <item x="166"/>
+        <item x="167"/>
+        <item x="332"/>
+        <item x="168"/>
+        <item x="169"/>
+        <item x="333"/>
+        <item x="334"/>
+        <item x="354"/>
+        <item x="335"/>
+        <item x="336"/>
+        <item x="337"/>
+        <item x="338"/>
+        <item x="170"/>
+        <item x="355"/>
+        <item x="339"/>
+        <item x="171"/>
+        <item x="340"/>
+        <item x="172"/>
+        <item x="356"/>
+        <item x="341"/>
+        <item x="342"/>
+        <item x="357"/>
+        <item x="343"/>
+        <item x="344"/>
+        <item x="147"/>
+        <item x="148"/>
+        <item x="173"/>
+        <item x="345"/>
+        <item x="358"/>
+        <item x="174"/>
+        <item x="149"/>
+        <item x="175"/>
+        <item x="176"/>
+        <item x="150"/>
+        <item x="359"/>
+        <item x="177"/>
+        <item x="346"/>
+        <item x="151"/>
+        <item x="360"/>
+        <item x="361"/>
+        <item x="362"/>
+        <item x="178"/>
+        <item x="152"/>
+        <item x="153"/>
+        <item x="363"/>
+        <item x="347"/>
+        <item x="154"/>
+        <item x="348"/>
+        <item x="364"/>
+        <item x="179"/>
+        <item x="180"/>
+        <item x="181"/>
+        <item x="349"/>
+        <item x="155"/>
+        <item x="156"/>
+        <item x="365"/>
+        <item x="366"/>
+        <item x="371"/>
+        <item x="372"/>
+        <item x="373"/>
+        <item x="374"/>
+        <item x="375"/>
+        <item x="376"/>
+        <item x="377"/>
+        <item x="378"/>
+        <item x="379"/>
+        <item x="380"/>
+        <item x="381"/>
+        <item x="382"/>
+        <item x="383"/>
+        <item x="384"/>
+        <item x="385"/>
+        <item x="386"/>
+        <item x="387"/>
+        <item x="388"/>
+        <item x="389"/>
+        <item x="390"/>
+        <item x="391"/>
+        <item x="392"/>
+        <item x="393"/>
+        <item x="394"/>
+        <item x="395"/>
+        <item x="396"/>
+        <item x="397"/>
+        <item x="398"/>
+        <item x="399"/>
+        <item x="400"/>
+        <item x="401"/>
+        <item x="402"/>
+        <item x="403"/>
+        <item x="404"/>
+        <item x="405"/>
+        <item x="406"/>
+        <item x="407"/>
+        <item x="408"/>
+        <item x="409"/>
+        <item x="410"/>
+        <item x="411"/>
+        <item x="412"/>
+        <item x="413"/>
+        <item x="414"/>
+        <item x="415"/>
+        <item x="416"/>
+        <item x="417"/>
+        <item x="418"/>
+        <item x="419"/>
+        <item x="420"/>
+        <item x="421"/>
+        <item x="422"/>
+        <item x="423"/>
+        <item x="424"/>
+        <item x="425"/>
+        <item x="426"/>
+        <item x="427"/>
+        <item x="428"/>
+        <item x="429"/>
+        <item x="430"/>
+        <item x="431"/>
+        <item x="432"/>
+        <item x="433"/>
+        <item x="434"/>
+        <item x="435"/>
+        <item x="436"/>
+        <item x="437"/>
+        <item x="438"/>
+        <item x="439"/>
+        <item x="440"/>
+        <item x="441"/>
+        <item x="442"/>
+        <item x="443"/>
+        <item x="444"/>
+        <item x="445"/>
+        <item x="446"/>
+        <item x="447"/>
+        <item x="448"/>
+        <item x="449"/>
+        <item x="450"/>
+        <item x="451"/>
+        <item x="452"/>
+        <item x="453"/>
+        <item x="454"/>
+        <item x="455"/>
+        <item x="456"/>
+        <item x="457"/>
+        <item x="458"/>
+        <item x="459"/>
+        <item x="460"/>
+        <item x="461"/>
+        <item x="462"/>
+        <item x="463"/>
+        <item x="464"/>
+        <item x="465"/>
+        <item x="466"/>
+        <item x="467"/>
+        <item x="468"/>
+        <item x="469"/>
+        <item x="470"/>
+        <item x="471"/>
+        <item x="472"/>
+        <item x="473"/>
+        <item x="474"/>
+        <item x="475"/>
+        <item x="476"/>
+        <item x="477"/>
+        <item x="478"/>
+        <item x="479"/>
+        <item x="480"/>
+        <item x="481"/>
+        <item x="482"/>
+        <item x="483"/>
+        <item x="484"/>
+        <item x="485"/>
+        <item x="486"/>
+        <item x="487"/>
+        <item x="488"/>
+        <item x="489"/>
+        <item x="490"/>
+        <item x="491"/>
+        <item x="492"/>
+        <item x="493"/>
+        <item x="494"/>
+        <item x="495"/>
+        <item x="496"/>
+        <item x="497"/>
+        <item x="498"/>
+        <item x="499"/>
+        <item x="500"/>
+        <item x="501"/>
+        <item x="502"/>
+        <item x="503"/>
+        <item x="504"/>
+        <item x="505"/>
+        <item x="506"/>
+        <item x="507"/>
+        <item x="508"/>
+        <item x="509"/>
+        <item x="510"/>
+        <item x="511"/>
+        <item x="512"/>
+        <item x="513"/>
+        <item x="514"/>
+        <item x="515"/>
+        <item x="516"/>
+        <item x="517"/>
+        <item x="518"/>
+        <item x="519"/>
+        <item x="520"/>
+        <item x="521"/>
+        <item x="522"/>
+        <item x="523"/>
+        <item x="524"/>
+        <item x="525"/>
+        <item x="526"/>
+        <item x="527"/>
+        <item x="528"/>
+        <item x="529"/>
+        <item x="530"/>
+        <item x="531"/>
+        <item x="532"/>
+        <item x="533"/>
+        <item x="534"/>
+        <item x="535"/>
+        <item x="536"/>
+        <item x="537"/>
+        <item x="538"/>
+        <item x="539"/>
+        <item x="540"/>
+        <item x="541"/>
+        <item x="542"/>
+        <item x="543"/>
+        <item x="544"/>
+        <item x="545"/>
+        <item x="546"/>
+        <item x="547"/>
+        <item x="548"/>
+        <item x="549"/>
+        <item x="550"/>
+        <item x="551"/>
+        <item x="552"/>
+        <item x="553"/>
+        <item x="554"/>
+        <item x="555"/>
+        <item x="556"/>
+        <item x="557"/>
+        <item x="558"/>
+        <item x="559"/>
+        <item x="560"/>
+        <item x="561"/>
+        <item x="562"/>
+        <item x="563"/>
+        <item x="564"/>
+        <item x="565"/>
+        <item x="566"/>
+        <item x="567"/>
+        <item x="568"/>
+        <item x="569"/>
+        <item x="570"/>
+        <item x="571"/>
+        <item x="572"/>
+        <item x="573"/>
+        <item x="574"/>
+        <item x="575"/>
+        <item x="576"/>
+        <item x="577"/>
+        <item x="578"/>
+        <item x="579"/>
+        <item x="580"/>
+        <item x="581"/>
+        <item x="582"/>
+        <item x="583"/>
+        <item x="584"/>
+        <item x="585"/>
+        <item x="586"/>
+        <item x="587"/>
+        <item x="588"/>
+        <item x="589"/>
+        <item x="590"/>
+        <item x="591"/>
+        <item x="592"/>
+        <item x="593"/>
+        <item x="594"/>
+        <item x="595"/>
+        <item x="596"/>
+        <item x="597"/>
+        <item x="598"/>
+        <item x="599"/>
+        <item x="600"/>
+        <item x="601"/>
+        <item x="602"/>
+        <item x="603"/>
+        <item x="604"/>
+        <item x="605"/>
+        <item x="606"/>
+        <item x="607"/>
+        <item x="608"/>
+        <item x="609"/>
+        <item x="610"/>
+        <item x="611"/>
+        <item x="612"/>
+        <item x="613"/>
+        <item x="614"/>
+        <item x="615"/>
+        <item x="616"/>
+        <item x="617"/>
+        <item x="618"/>
+        <item x="619"/>
+        <item x="620"/>
+        <item x="621"/>
+        <item x="622"/>
+        <item x="623"/>
+        <item x="624"/>
+        <item x="625"/>
+        <item x="626"/>
+        <item x="627"/>
+        <item x="628"/>
+        <item x="629"/>
+        <item x="630"/>
+        <item x="631"/>
+        <item x="632"/>
+        <item x="633"/>
+        <item x="634"/>
+        <item x="635"/>
+        <item x="636"/>
+        <item x="637"/>
+        <item x="638"/>
+        <item x="639"/>
+        <item x="640"/>
+        <item x="641"/>
+        <item x="642"/>
+        <item x="643"/>
+        <item x="644"/>
+        <item x="645"/>
+        <item x="646"/>
+        <item x="647"/>
+        <item x="648"/>
+        <item x="649"/>
+        <item x="650"/>
+        <item x="651"/>
+        <item x="652"/>
+        <item x="653"/>
+        <item x="654"/>
+        <item x="655"/>
+        <item x="656"/>
+        <item x="657"/>
+        <item x="658"/>
+        <item x="659"/>
+        <item x="660"/>
+        <item x="661"/>
+        <item x="662"/>
+        <item x="663"/>
+        <item x="664"/>
+        <item x="665"/>
+        <item x="666"/>
+        <item x="667"/>
+        <item x="668"/>
+        <item x="669"/>
+        <item x="670"/>
+        <item x="671"/>
+        <item x="672"/>
+        <item x="673"/>
+        <item x="674"/>
+        <item x="675"/>
+        <item x="676"/>
+        <item x="677"/>
+        <item x="678"/>
+        <item x="679"/>
+        <item x="680"/>
+        <item x="681"/>
+        <item x="682"/>
+        <item x="683"/>
+        <item x="684"/>
+        <item x="685"/>
+        <item x="686"/>
+        <item x="687"/>
+        <item x="688"/>
+        <item x="689"/>
+        <item x="690"/>
+        <item x="691"/>
+        <item x="692"/>
+        <item x="693"/>
+        <item x="694"/>
+        <item x="695"/>
+        <item x="696"/>
+        <item x="697"/>
+        <item x="698"/>
+        <item x="699"/>
+        <item x="700"/>
+        <item x="701"/>
+        <item x="702"/>
+        <item x="703"/>
+        <item x="704"/>
+        <item x="705"/>
+        <item x="706"/>
+        <item x="707"/>
+        <item x="708"/>
+        <item x="709"/>
+        <item x="710"/>
+        <item x="711"/>
+        <item x="712"/>
+        <item x="713"/>
+        <item x="714"/>
+        <item x="715"/>
+        <item x="716"/>
+        <item x="717"/>
+        <item x="718"/>
+        <item x="719"/>
+        <item x="720"/>
+        <item x="721"/>
+        <item x="722"/>
+        <item x="723"/>
+        <item x="724"/>
+        <item x="725"/>
+        <item x="726"/>
+        <item x="727"/>
+        <item x="728"/>
+        <item x="729"/>
+        <item x="730"/>
+        <item x="731"/>
+        <item x="732"/>
+        <item x="733"/>
+        <item x="734"/>
+        <item x="735"/>
+        <item x="736"/>
+        <item x="737"/>
+        <item x="738"/>
+        <item x="739"/>
+        <item x="740"/>
+        <item x="741"/>
+        <item x="742"/>
+        <item x="743"/>
+        <item x="744"/>
+        <item x="745"/>
+        <item x="746"/>
+        <item x="747"/>
+        <item x="748"/>
+        <item x="749"/>
+        <item x="750"/>
+        <item x="751"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Max of identifier " fld="0" subtotal="max" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{47F20B7A-000C-470D-AB36-BE8093AA4DE3}" name="PivotTable16" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A13:A14" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" showAll="0">
+      <items count="753">
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="207"/>
+        <item x="208"/>
+        <item x="209"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="210"/>
+        <item x="211"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="212"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="213"/>
+        <item x="33"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="182"/>
+        <item x="34"/>
+        <item x="214"/>
+        <item x="35"/>
+        <item x="183"/>
+        <item x="184"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="36"/>
+        <item x="185"/>
+        <item x="215"/>
+        <item x="186"/>
+        <item x="187"/>
+        <item x="37"/>
+        <item x="216"/>
+        <item x="188"/>
+        <item x="189"/>
+        <item x="217"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="190"/>
+        <item x="218"/>
+        <item x="191"/>
+        <item x="219"/>
+        <item x="40"/>
+        <item x="220"/>
+        <item x="41"/>
+        <item x="221"/>
+        <item x="6"/>
+        <item x="42"/>
+        <item x="192"/>
+        <item x="193"/>
+        <item x="43"/>
+        <item x="222"/>
+        <item x="44"/>
+        <item x="7"/>
+        <item x="194"/>
+        <item x="45"/>
+        <item x="8"/>
+        <item x="223"/>
+        <item x="224"/>
+        <item x="46"/>
+        <item x="225"/>
+        <item x="47"/>
+        <item x="195"/>
+        <item x="226"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="227"/>
+        <item x="228"/>
+        <item x="229"/>
+        <item x="230"/>
+        <item x="9"/>
+        <item x="50"/>
+        <item x="196"/>
+        <item x="197"/>
+        <item x="231"/>
+        <item x="232"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="198"/>
+        <item x="233"/>
+        <item x="199"/>
+        <item x="234"/>
+        <item x="200"/>
+        <item x="69"/>
+        <item x="235"/>
+        <item x="201"/>
+        <item x="10"/>
+        <item x="70"/>
+        <item x="11"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="202"/>
+        <item x="249"/>
+        <item x="250"/>
+        <item x="251"/>
+        <item x="203"/>
+        <item x="204"/>
+        <item x="73"/>
+        <item x="12"/>
+        <item x="252"/>
+        <item x="13"/>
+        <item x="74"/>
+        <item x="253"/>
+        <item x="205"/>
+        <item x="75"/>
+        <item x="14"/>
+        <item x="206"/>
+        <item x="236"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="51"/>
+        <item x="254"/>
+        <item x="78"/>
+        <item x="52"/>
+        <item x="79"/>
+        <item x="53"/>
+        <item x="237"/>
+        <item x="80"/>
+        <item x="54"/>
+        <item x="81"/>
+        <item x="255"/>
+        <item x="256"/>
+        <item x="257"/>
+        <item x="238"/>
+        <item x="258"/>
+        <item x="82"/>
+        <item x="239"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="259"/>
+        <item x="240"/>
+        <item x="241"/>
+        <item x="83"/>
+        <item x="260"/>
+        <item x="242"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="243"/>
+        <item x="57"/>
+        <item x="86"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="244"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="89"/>
+        <item x="261"/>
+        <item x="90"/>
+        <item x="62"/>
+        <item x="262"/>
+        <item x="63"/>
+        <item x="245"/>
+        <item x="246"/>
+        <item x="64"/>
+        <item x="91"/>
+        <item x="263"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="92"/>
+        <item x="93"/>
+        <item x="247"/>
+        <item x="264"/>
+        <item x="265"/>
+        <item x="97"/>
+        <item x="266"/>
+        <item x="248"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item x="100"/>
+        <item x="284"/>
+        <item x="101"/>
+        <item x="102"/>
+        <item x="285"/>
+        <item x="94"/>
+        <item x="286"/>
+        <item x="287"/>
+        <item x="288"/>
+        <item x="267"/>
+        <item x="268"/>
+        <item x="289"/>
+        <item x="103"/>
+        <item x="269"/>
+        <item x="104"/>
+        <item x="270"/>
+        <item x="95"/>
+        <item x="271"/>
+        <item x="272"/>
+        <item x="96"/>
+        <item x="273"/>
+        <item x="105"/>
+        <item x="274"/>
+        <item x="290"/>
+        <item x="106"/>
+        <item x="291"/>
+        <item x="275"/>
+        <item x="292"/>
+        <item x="107"/>
+        <item x="108"/>
+        <item x="276"/>
+        <item x="277"/>
+        <item x="293"/>
+        <item x="278"/>
+        <item x="279"/>
+        <item x="280"/>
+        <item x="294"/>
+        <item x="300"/>
+        <item x="281"/>
+        <item x="117"/>
+        <item x="118"/>
+        <item x="282"/>
+        <item x="301"/>
+        <item x="283"/>
+        <item x="302"/>
+        <item x="119"/>
+        <item x="295"/>
+        <item x="120"/>
+        <item x="303"/>
+        <item x="296"/>
+        <item x="297"/>
+        <item x="109"/>
+        <item x="298"/>
+        <item x="304"/>
+        <item x="305"/>
+        <item x="110"/>
+        <item x="299"/>
+        <item x="306"/>
+        <item x="124"/>
+        <item x="125"/>
+        <item x="310"/>
+        <item x="111"/>
+        <item x="126"/>
+        <item x="127"/>
+        <item x="112"/>
+        <item x="136"/>
+        <item x="113"/>
+        <item x="114"/>
+        <item x="115"/>
+        <item x="116"/>
+        <item x="307"/>
+        <item x="131"/>
+        <item x="308"/>
+        <item x="121"/>
+        <item x="132"/>
+        <item x="311"/>
+        <item x="133"/>
+        <item x="122"/>
+        <item x="137"/>
+        <item x="138"/>
+        <item x="367"/>
+        <item x="312"/>
+        <item x="123"/>
+        <item x="317"/>
+        <item x="318"/>
+        <item x="309"/>
+        <item x="313"/>
+        <item x="128"/>
+        <item x="319"/>
+        <item x="314"/>
+        <item x="129"/>
+        <item x="315"/>
+        <item x="130"/>
+        <item x="320"/>
+        <item x="316"/>
+        <item x="141"/>
+        <item x="142"/>
+        <item x="145"/>
+        <item x="134"/>
+        <item x="146"/>
+        <item x="321"/>
+        <item x="325"/>
+        <item x="322"/>
+        <item x="323"/>
+        <item x="135"/>
+        <item x="326"/>
+        <item x="327"/>
+        <item x="368"/>
+        <item x="139"/>
+        <item x="140"/>
+        <item x="157"/>
+        <item x="158"/>
+        <item x="324"/>
+        <item x="159"/>
+        <item x="328"/>
+        <item x="329"/>
+        <item x="160"/>
+        <item x="369"/>
+        <item x="161"/>
+        <item x="162"/>
+        <item x="143"/>
+        <item x="144"/>
+        <item x="330"/>
+        <item x="350"/>
+        <item x="351"/>
+        <item x="370"/>
+        <item x="163"/>
+        <item x="352"/>
+        <item x="164"/>
+        <item x="331"/>
+        <item x="353"/>
+        <item x="165"/>
+        <item x="166"/>
+        <item x="167"/>
+        <item x="332"/>
+        <item x="168"/>
+        <item x="169"/>
+        <item x="333"/>
+        <item x="334"/>
+        <item x="354"/>
+        <item x="335"/>
+        <item x="336"/>
+        <item x="337"/>
+        <item x="338"/>
+        <item x="170"/>
+        <item x="355"/>
+        <item x="339"/>
+        <item x="171"/>
+        <item x="340"/>
+        <item x="172"/>
+        <item x="356"/>
+        <item x="341"/>
+        <item x="342"/>
+        <item x="357"/>
+        <item x="343"/>
+        <item x="344"/>
+        <item x="147"/>
+        <item x="148"/>
+        <item x="173"/>
+        <item x="345"/>
+        <item x="358"/>
+        <item x="174"/>
+        <item x="149"/>
+        <item x="175"/>
+        <item x="176"/>
+        <item x="150"/>
+        <item x="359"/>
+        <item x="177"/>
+        <item x="346"/>
+        <item x="151"/>
+        <item x="360"/>
+        <item x="361"/>
+        <item x="362"/>
+        <item x="178"/>
+        <item x="152"/>
+        <item x="153"/>
+        <item x="363"/>
+        <item x="347"/>
+        <item x="154"/>
+        <item x="348"/>
+        <item x="364"/>
+        <item x="179"/>
+        <item x="180"/>
+        <item x="181"/>
+        <item x="349"/>
+        <item x="155"/>
+        <item x="156"/>
+        <item x="365"/>
+        <item x="366"/>
+        <item x="371"/>
+        <item x="372"/>
+        <item x="373"/>
+        <item x="374"/>
+        <item x="375"/>
+        <item x="376"/>
+        <item x="377"/>
+        <item x="378"/>
+        <item x="379"/>
+        <item x="380"/>
+        <item x="381"/>
+        <item x="382"/>
+        <item x="383"/>
+        <item x="384"/>
+        <item x="385"/>
+        <item x="386"/>
+        <item x="387"/>
+        <item x="388"/>
+        <item x="389"/>
+        <item x="390"/>
+        <item x="391"/>
+        <item x="392"/>
+        <item x="393"/>
+        <item x="394"/>
+        <item x="395"/>
+        <item x="396"/>
+        <item x="397"/>
+        <item x="398"/>
+        <item x="399"/>
+        <item x="400"/>
+        <item x="401"/>
+        <item x="402"/>
+        <item x="403"/>
+        <item x="404"/>
+        <item x="405"/>
+        <item x="406"/>
+        <item x="407"/>
+        <item x="408"/>
+        <item x="409"/>
+        <item x="410"/>
+        <item x="411"/>
+        <item x="412"/>
+        <item x="413"/>
+        <item x="414"/>
+        <item x="415"/>
+        <item x="416"/>
+        <item x="417"/>
+        <item x="418"/>
+        <item x="419"/>
+        <item x="420"/>
+        <item x="421"/>
+        <item x="422"/>
+        <item x="423"/>
+        <item x="424"/>
+        <item x="425"/>
+        <item x="426"/>
+        <item x="427"/>
+        <item x="428"/>
+        <item x="429"/>
+        <item x="430"/>
+        <item x="431"/>
+        <item x="432"/>
+        <item x="433"/>
+        <item x="434"/>
+        <item x="435"/>
+        <item x="436"/>
+        <item x="437"/>
+        <item x="438"/>
+        <item x="439"/>
+        <item x="440"/>
+        <item x="441"/>
+        <item x="442"/>
+        <item x="443"/>
+        <item x="444"/>
+        <item x="445"/>
+        <item x="446"/>
+        <item x="447"/>
+        <item x="448"/>
+        <item x="449"/>
+        <item x="450"/>
+        <item x="451"/>
+        <item x="452"/>
+        <item x="453"/>
+        <item x="454"/>
+        <item x="455"/>
+        <item x="456"/>
+        <item x="457"/>
+        <item x="458"/>
+        <item x="459"/>
+        <item x="460"/>
+        <item x="461"/>
+        <item x="462"/>
+        <item x="463"/>
+        <item x="464"/>
+        <item x="465"/>
+        <item x="466"/>
+        <item x="467"/>
+        <item x="468"/>
+        <item x="469"/>
+        <item x="470"/>
+        <item x="471"/>
+        <item x="472"/>
+        <item x="473"/>
+        <item x="474"/>
+        <item x="475"/>
+        <item x="476"/>
+        <item x="477"/>
+        <item x="478"/>
+        <item x="479"/>
+        <item x="480"/>
+        <item x="481"/>
+        <item x="482"/>
+        <item x="483"/>
+        <item x="484"/>
+        <item x="485"/>
+        <item x="486"/>
+        <item x="487"/>
+        <item x="488"/>
+        <item x="489"/>
+        <item x="490"/>
+        <item x="491"/>
+        <item x="492"/>
+        <item x="493"/>
+        <item x="494"/>
+        <item x="495"/>
+        <item x="496"/>
+        <item x="497"/>
+        <item x="498"/>
+        <item x="499"/>
+        <item x="500"/>
+        <item x="501"/>
+        <item x="502"/>
+        <item x="503"/>
+        <item x="504"/>
+        <item x="505"/>
+        <item x="506"/>
+        <item x="507"/>
+        <item x="508"/>
+        <item x="509"/>
+        <item x="510"/>
+        <item x="511"/>
+        <item x="512"/>
+        <item x="513"/>
+        <item x="514"/>
+        <item x="515"/>
+        <item x="516"/>
+        <item x="517"/>
+        <item x="518"/>
+        <item x="519"/>
+        <item x="520"/>
+        <item x="521"/>
+        <item x="522"/>
+        <item x="523"/>
+        <item x="524"/>
+        <item x="525"/>
+        <item x="526"/>
+        <item x="527"/>
+        <item x="528"/>
+        <item x="529"/>
+        <item x="530"/>
+        <item x="531"/>
+        <item x="532"/>
+        <item x="533"/>
+        <item x="534"/>
+        <item x="535"/>
+        <item x="536"/>
+        <item x="537"/>
+        <item x="538"/>
+        <item x="539"/>
+        <item x="540"/>
+        <item x="541"/>
+        <item x="542"/>
+        <item x="543"/>
+        <item x="544"/>
+        <item x="545"/>
+        <item x="546"/>
+        <item x="547"/>
+        <item x="548"/>
+        <item x="549"/>
+        <item x="550"/>
+        <item x="551"/>
+        <item x="552"/>
+        <item x="553"/>
+        <item x="554"/>
+        <item x="555"/>
+        <item x="556"/>
+        <item x="557"/>
+        <item x="558"/>
+        <item x="559"/>
+        <item x="560"/>
+        <item x="561"/>
+        <item x="562"/>
+        <item x="563"/>
+        <item x="564"/>
+        <item x="565"/>
+        <item x="566"/>
+        <item x="567"/>
+        <item x="568"/>
+        <item x="569"/>
+        <item x="570"/>
+        <item x="571"/>
+        <item x="572"/>
+        <item x="573"/>
+        <item x="574"/>
+        <item x="575"/>
+        <item x="576"/>
+        <item x="577"/>
+        <item x="578"/>
+        <item x="579"/>
+        <item x="580"/>
+        <item x="581"/>
+        <item x="582"/>
+        <item x="583"/>
+        <item x="584"/>
+        <item x="585"/>
+        <item x="586"/>
+        <item x="587"/>
+        <item x="588"/>
+        <item x="589"/>
+        <item x="590"/>
+        <item x="591"/>
+        <item x="592"/>
+        <item x="593"/>
+        <item x="594"/>
+        <item x="595"/>
+        <item x="596"/>
+        <item x="597"/>
+        <item x="598"/>
+        <item x="599"/>
+        <item x="600"/>
+        <item x="601"/>
+        <item x="602"/>
+        <item x="603"/>
+        <item x="604"/>
+        <item x="605"/>
+        <item x="606"/>
+        <item x="607"/>
+        <item x="608"/>
+        <item x="609"/>
+        <item x="610"/>
+        <item x="611"/>
+        <item x="612"/>
+        <item x="613"/>
+        <item x="614"/>
+        <item x="615"/>
+        <item x="616"/>
+        <item x="617"/>
+        <item x="618"/>
+        <item x="619"/>
+        <item x="620"/>
+        <item x="621"/>
+        <item x="622"/>
+        <item x="623"/>
+        <item x="624"/>
+        <item x="625"/>
+        <item x="626"/>
+        <item x="627"/>
+        <item x="628"/>
+        <item x="629"/>
+        <item x="630"/>
+        <item x="631"/>
+        <item x="632"/>
+        <item x="633"/>
+        <item x="634"/>
+        <item x="635"/>
+        <item x="636"/>
+        <item x="637"/>
+        <item x="638"/>
+        <item x="639"/>
+        <item x="640"/>
+        <item x="641"/>
+        <item x="642"/>
+        <item x="643"/>
+        <item x="644"/>
+        <item x="645"/>
+        <item x="646"/>
+        <item x="647"/>
+        <item x="648"/>
+        <item x="649"/>
+        <item x="650"/>
+        <item x="651"/>
+        <item x="652"/>
+        <item x="653"/>
+        <item x="654"/>
+        <item x="655"/>
+        <item x="656"/>
+        <item x="657"/>
+        <item x="658"/>
+        <item x="659"/>
+        <item x="660"/>
+        <item x="661"/>
+        <item x="662"/>
+        <item x="663"/>
+        <item x="664"/>
+        <item x="665"/>
+        <item x="666"/>
+        <item x="667"/>
+        <item x="668"/>
+        <item x="669"/>
+        <item x="670"/>
+        <item x="671"/>
+        <item x="672"/>
+        <item x="673"/>
+        <item x="674"/>
+        <item x="675"/>
+        <item x="676"/>
+        <item x="677"/>
+        <item x="678"/>
+        <item x="679"/>
+        <item x="680"/>
+        <item x="681"/>
+        <item x="682"/>
+        <item x="683"/>
+        <item x="684"/>
+        <item x="685"/>
+        <item x="686"/>
+        <item x="687"/>
+        <item x="688"/>
+        <item x="689"/>
+        <item x="690"/>
+        <item x="691"/>
+        <item x="692"/>
+        <item x="693"/>
+        <item x="694"/>
+        <item x="695"/>
+        <item x="696"/>
+        <item x="697"/>
+        <item x="698"/>
+        <item x="699"/>
+        <item x="700"/>
+        <item x="701"/>
+        <item x="702"/>
+        <item x="703"/>
+        <item x="704"/>
+        <item x="705"/>
+        <item x="706"/>
+        <item x="707"/>
+        <item x="708"/>
+        <item x="709"/>
+        <item x="710"/>
+        <item x="711"/>
+        <item x="712"/>
+        <item x="713"/>
+        <item x="714"/>
+        <item x="715"/>
+        <item x="716"/>
+        <item x="717"/>
+        <item x="718"/>
+        <item x="719"/>
+        <item x="720"/>
+        <item x="721"/>
+        <item x="722"/>
+        <item x="723"/>
+        <item x="724"/>
+        <item x="725"/>
+        <item x="726"/>
+        <item x="727"/>
+        <item x="728"/>
+        <item x="729"/>
+        <item x="730"/>
+        <item x="731"/>
+        <item x="732"/>
+        <item x="733"/>
+        <item x="734"/>
+        <item x="735"/>
+        <item x="736"/>
+        <item x="737"/>
+        <item x="738"/>
+        <item x="739"/>
+        <item x="740"/>
+        <item x="741"/>
+        <item x="742"/>
+        <item x="743"/>
+        <item x="744"/>
+        <item x="745"/>
+        <item x="746"/>
+        <item x="747"/>
+        <item x="748"/>
+        <item x="749"/>
+        <item x="750"/>
+        <item x="751"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Min of identifier " fld="0" subtotal="min" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{554892DA-28FD-4713-9225-4AEE1188F6D2}" name="PivotTable15" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A23:A24" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="4">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Max of identifier " fld="0" subtotal="max" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C2C0A457-DB5D-46F8-9958-EBDCB218DBEC}" name="PivotTable14" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A21:A22" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="4">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Min of identifier " fld="0" subtotal="min" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{779D602B-5C6E-485C-9366-F1ACB9C4DC86}" name="PivotTable12" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A18:A19" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="4">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of identifier " fld="0" subtotal="count" baseField="1" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9469789E-4256-4AA3-824B-32C42216DDD3}" name="PivotTable11" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A10:A11" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" showAll="0">
+      <items count="753">
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="207"/>
+        <item x="208"/>
+        <item x="209"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="210"/>
+        <item x="211"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="212"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="213"/>
+        <item x="33"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="182"/>
+        <item x="34"/>
+        <item x="214"/>
+        <item x="35"/>
+        <item x="183"/>
+        <item x="184"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="36"/>
+        <item x="185"/>
+        <item x="215"/>
+        <item x="186"/>
+        <item x="187"/>
+        <item x="37"/>
+        <item x="216"/>
+        <item x="188"/>
+        <item x="189"/>
+        <item x="217"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="190"/>
+        <item x="218"/>
+        <item x="191"/>
+        <item x="219"/>
+        <item x="40"/>
+        <item x="220"/>
+        <item x="41"/>
+        <item x="221"/>
+        <item x="6"/>
+        <item x="42"/>
+        <item x="192"/>
+        <item x="193"/>
+        <item x="43"/>
+        <item x="222"/>
+        <item x="44"/>
+        <item x="7"/>
+        <item x="194"/>
+        <item x="45"/>
+        <item x="8"/>
+        <item x="223"/>
+        <item x="224"/>
+        <item x="46"/>
+        <item x="225"/>
+        <item x="47"/>
+        <item x="195"/>
+        <item x="226"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="227"/>
+        <item x="228"/>
+        <item x="229"/>
+        <item x="230"/>
+        <item x="9"/>
+        <item x="50"/>
+        <item x="196"/>
+        <item x="197"/>
+        <item x="231"/>
+        <item x="232"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="198"/>
+        <item x="233"/>
+        <item x="199"/>
+        <item x="234"/>
+        <item x="200"/>
+        <item x="69"/>
+        <item x="235"/>
+        <item x="201"/>
+        <item x="10"/>
+        <item x="70"/>
+        <item x="11"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="202"/>
+        <item x="249"/>
+        <item x="250"/>
+        <item x="251"/>
+        <item x="203"/>
+        <item x="204"/>
+        <item x="73"/>
+        <item x="12"/>
+        <item x="252"/>
+        <item x="13"/>
+        <item x="74"/>
+        <item x="253"/>
+        <item x="205"/>
+        <item x="75"/>
+        <item x="14"/>
+        <item x="206"/>
+        <item x="236"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="51"/>
+        <item x="254"/>
+        <item x="78"/>
+        <item x="52"/>
+        <item x="79"/>
+        <item x="53"/>
+        <item x="237"/>
+        <item x="80"/>
+        <item x="54"/>
+        <item x="81"/>
+        <item x="255"/>
+        <item x="256"/>
+        <item x="257"/>
+        <item x="238"/>
+        <item x="258"/>
+        <item x="82"/>
+        <item x="239"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="259"/>
+        <item x="240"/>
+        <item x="241"/>
+        <item x="83"/>
+        <item x="260"/>
+        <item x="242"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="243"/>
+        <item x="57"/>
+        <item x="86"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="244"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="89"/>
+        <item x="261"/>
+        <item x="90"/>
+        <item x="62"/>
+        <item x="262"/>
+        <item x="63"/>
+        <item x="245"/>
+        <item x="246"/>
+        <item x="64"/>
+        <item x="91"/>
+        <item x="263"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="92"/>
+        <item x="93"/>
+        <item x="247"/>
+        <item x="264"/>
+        <item x="265"/>
+        <item x="97"/>
+        <item x="266"/>
+        <item x="248"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item x="100"/>
+        <item x="284"/>
+        <item x="101"/>
+        <item x="102"/>
+        <item x="285"/>
+        <item x="94"/>
+        <item x="286"/>
+        <item x="287"/>
+        <item x="288"/>
+        <item x="267"/>
+        <item x="268"/>
+        <item x="289"/>
+        <item x="103"/>
+        <item x="269"/>
+        <item x="104"/>
+        <item x="270"/>
+        <item x="95"/>
+        <item x="271"/>
+        <item x="272"/>
+        <item x="96"/>
+        <item x="273"/>
+        <item x="105"/>
+        <item x="274"/>
+        <item x="290"/>
+        <item x="106"/>
+        <item x="291"/>
+        <item x="275"/>
+        <item x="292"/>
+        <item x="107"/>
+        <item x="108"/>
+        <item x="276"/>
+        <item x="277"/>
+        <item x="293"/>
+        <item x="278"/>
+        <item x="279"/>
+        <item x="280"/>
+        <item x="294"/>
+        <item x="300"/>
+        <item x="281"/>
+        <item x="117"/>
+        <item x="118"/>
+        <item x="282"/>
+        <item x="301"/>
+        <item x="283"/>
+        <item x="302"/>
+        <item x="119"/>
+        <item x="295"/>
+        <item x="120"/>
+        <item x="303"/>
+        <item x="296"/>
+        <item x="297"/>
+        <item x="109"/>
+        <item x="298"/>
+        <item x="304"/>
+        <item x="305"/>
+        <item x="110"/>
+        <item x="299"/>
+        <item x="306"/>
+        <item x="124"/>
+        <item x="125"/>
+        <item x="310"/>
+        <item x="111"/>
+        <item x="126"/>
+        <item x="127"/>
+        <item x="112"/>
+        <item x="136"/>
+        <item x="113"/>
+        <item x="114"/>
+        <item x="115"/>
+        <item x="116"/>
+        <item x="307"/>
+        <item x="131"/>
+        <item x="308"/>
+        <item x="121"/>
+        <item x="132"/>
+        <item x="311"/>
+        <item x="133"/>
+        <item x="122"/>
+        <item x="137"/>
+        <item x="138"/>
+        <item x="367"/>
+        <item x="312"/>
+        <item x="123"/>
+        <item x="317"/>
+        <item x="318"/>
+        <item x="309"/>
+        <item x="313"/>
+        <item x="128"/>
+        <item x="319"/>
+        <item x="314"/>
+        <item x="129"/>
+        <item x="315"/>
+        <item x="130"/>
+        <item x="320"/>
+        <item x="316"/>
+        <item x="141"/>
+        <item x="142"/>
+        <item x="145"/>
+        <item x="134"/>
+        <item x="146"/>
+        <item x="321"/>
+        <item x="325"/>
+        <item x="322"/>
+        <item x="323"/>
+        <item x="135"/>
+        <item x="326"/>
+        <item x="327"/>
+        <item x="368"/>
+        <item x="139"/>
+        <item x="140"/>
+        <item x="157"/>
+        <item x="158"/>
+        <item x="324"/>
+        <item x="159"/>
+        <item x="328"/>
+        <item x="329"/>
+        <item x="160"/>
+        <item x="369"/>
+        <item x="161"/>
+        <item x="162"/>
+        <item x="143"/>
+        <item x="144"/>
+        <item x="330"/>
+        <item x="350"/>
+        <item x="351"/>
+        <item x="370"/>
+        <item x="163"/>
+        <item x="352"/>
+        <item x="164"/>
+        <item x="331"/>
+        <item x="353"/>
+        <item x="165"/>
+        <item x="166"/>
+        <item x="167"/>
+        <item x="332"/>
+        <item x="168"/>
+        <item x="169"/>
+        <item x="333"/>
+        <item x="334"/>
+        <item x="354"/>
+        <item x="335"/>
+        <item x="336"/>
+        <item x="337"/>
+        <item x="338"/>
+        <item x="170"/>
+        <item x="355"/>
+        <item x="339"/>
+        <item x="171"/>
+        <item x="340"/>
+        <item x="172"/>
+        <item x="356"/>
+        <item x="341"/>
+        <item x="342"/>
+        <item x="357"/>
+        <item x="343"/>
+        <item x="344"/>
+        <item x="147"/>
+        <item x="148"/>
+        <item x="173"/>
+        <item x="345"/>
+        <item x="358"/>
+        <item x="174"/>
+        <item x="149"/>
+        <item x="175"/>
+        <item x="176"/>
+        <item x="150"/>
+        <item x="359"/>
+        <item x="177"/>
+        <item x="346"/>
+        <item x="151"/>
+        <item x="360"/>
+        <item x="361"/>
+        <item x="362"/>
+        <item x="178"/>
+        <item x="152"/>
+        <item x="153"/>
+        <item x="363"/>
+        <item x="347"/>
+        <item x="154"/>
+        <item x="348"/>
+        <item x="364"/>
+        <item x="179"/>
+        <item x="180"/>
+        <item x="181"/>
+        <item x="349"/>
+        <item x="155"/>
+        <item x="156"/>
+        <item x="365"/>
+        <item x="366"/>
+        <item x="371"/>
+        <item x="372"/>
+        <item x="373"/>
+        <item x="374"/>
+        <item x="375"/>
+        <item x="376"/>
+        <item x="377"/>
+        <item x="378"/>
+        <item x="379"/>
+        <item x="380"/>
+        <item x="381"/>
+        <item x="382"/>
+        <item x="383"/>
+        <item x="384"/>
+        <item x="385"/>
+        <item x="386"/>
+        <item x="387"/>
+        <item x="388"/>
+        <item x="389"/>
+        <item x="390"/>
+        <item x="391"/>
+        <item x="392"/>
+        <item x="393"/>
+        <item x="394"/>
+        <item x="395"/>
+        <item x="396"/>
+        <item x="397"/>
+        <item x="398"/>
+        <item x="399"/>
+        <item x="400"/>
+        <item x="401"/>
+        <item x="402"/>
+        <item x="403"/>
+        <item x="404"/>
+        <item x="405"/>
+        <item x="406"/>
+        <item x="407"/>
+        <item x="408"/>
+        <item x="409"/>
+        <item x="410"/>
+        <item x="411"/>
+        <item x="412"/>
+        <item x="413"/>
+        <item x="414"/>
+        <item x="415"/>
+        <item x="416"/>
+        <item x="417"/>
+        <item x="418"/>
+        <item x="419"/>
+        <item x="420"/>
+        <item x="421"/>
+        <item x="422"/>
+        <item x="423"/>
+        <item x="424"/>
+        <item x="425"/>
+        <item x="426"/>
+        <item x="427"/>
+        <item x="428"/>
+        <item x="429"/>
+        <item x="430"/>
+        <item x="431"/>
+        <item x="432"/>
+        <item x="433"/>
+        <item x="434"/>
+        <item x="435"/>
+        <item x="436"/>
+        <item x="437"/>
+        <item x="438"/>
+        <item x="439"/>
+        <item x="440"/>
+        <item x="441"/>
+        <item x="442"/>
+        <item x="443"/>
+        <item x="444"/>
+        <item x="445"/>
+        <item x="446"/>
+        <item x="447"/>
+        <item x="448"/>
+        <item x="449"/>
+        <item x="450"/>
+        <item x="451"/>
+        <item x="452"/>
+        <item x="453"/>
+        <item x="454"/>
+        <item x="455"/>
+        <item x="456"/>
+        <item x="457"/>
+        <item x="458"/>
+        <item x="459"/>
+        <item x="460"/>
+        <item x="461"/>
+        <item x="462"/>
+        <item x="463"/>
+        <item x="464"/>
+        <item x="465"/>
+        <item x="466"/>
+        <item x="467"/>
+        <item x="468"/>
+        <item x="469"/>
+        <item x="470"/>
+        <item x="471"/>
+        <item x="472"/>
+        <item x="473"/>
+        <item x="474"/>
+        <item x="475"/>
+        <item x="476"/>
+        <item x="477"/>
+        <item x="478"/>
+        <item x="479"/>
+        <item x="480"/>
+        <item x="481"/>
+        <item x="482"/>
+        <item x="483"/>
+        <item x="484"/>
+        <item x="485"/>
+        <item x="486"/>
+        <item x="487"/>
+        <item x="488"/>
+        <item x="489"/>
+        <item x="490"/>
+        <item x="491"/>
+        <item x="492"/>
+        <item x="493"/>
+        <item x="494"/>
+        <item x="495"/>
+        <item x="496"/>
+        <item x="497"/>
+        <item x="498"/>
+        <item x="499"/>
+        <item x="500"/>
+        <item x="501"/>
+        <item x="502"/>
+        <item x="503"/>
+        <item x="504"/>
+        <item x="505"/>
+        <item x="506"/>
+        <item x="507"/>
+        <item x="508"/>
+        <item x="509"/>
+        <item x="510"/>
+        <item x="511"/>
+        <item x="512"/>
+        <item x="513"/>
+        <item x="514"/>
+        <item x="515"/>
+        <item x="516"/>
+        <item x="517"/>
+        <item x="518"/>
+        <item x="519"/>
+        <item x="520"/>
+        <item x="521"/>
+        <item x="522"/>
+        <item x="523"/>
+        <item x="524"/>
+        <item x="525"/>
+        <item x="526"/>
+        <item x="527"/>
+        <item x="528"/>
+        <item x="529"/>
+        <item x="530"/>
+        <item x="531"/>
+        <item x="532"/>
+        <item x="533"/>
+        <item x="534"/>
+        <item x="535"/>
+        <item x="536"/>
+        <item x="537"/>
+        <item x="538"/>
+        <item x="539"/>
+        <item x="540"/>
+        <item x="541"/>
+        <item x="542"/>
+        <item x="543"/>
+        <item x="544"/>
+        <item x="545"/>
+        <item x="546"/>
+        <item x="547"/>
+        <item x="548"/>
+        <item x="549"/>
+        <item x="550"/>
+        <item x="551"/>
+        <item x="552"/>
+        <item x="553"/>
+        <item x="554"/>
+        <item x="555"/>
+        <item x="556"/>
+        <item x="557"/>
+        <item x="558"/>
+        <item x="559"/>
+        <item x="560"/>
+        <item x="561"/>
+        <item x="562"/>
+        <item x="563"/>
+        <item x="564"/>
+        <item x="565"/>
+        <item x="566"/>
+        <item x="567"/>
+        <item x="568"/>
+        <item x="569"/>
+        <item x="570"/>
+        <item x="571"/>
+        <item x="572"/>
+        <item x="573"/>
+        <item x="574"/>
+        <item x="575"/>
+        <item x="576"/>
+        <item x="577"/>
+        <item x="578"/>
+        <item x="579"/>
+        <item x="580"/>
+        <item x="581"/>
+        <item x="582"/>
+        <item x="583"/>
+        <item x="584"/>
+        <item x="585"/>
+        <item x="586"/>
+        <item x="587"/>
+        <item x="588"/>
+        <item x="589"/>
+        <item x="590"/>
+        <item x="591"/>
+        <item x="592"/>
+        <item x="593"/>
+        <item x="594"/>
+        <item x="595"/>
+        <item x="596"/>
+        <item x="597"/>
+        <item x="598"/>
+        <item x="599"/>
+        <item x="600"/>
+        <item x="601"/>
+        <item x="602"/>
+        <item x="603"/>
+        <item x="604"/>
+        <item x="605"/>
+        <item x="606"/>
+        <item x="607"/>
+        <item x="608"/>
+        <item x="609"/>
+        <item x="610"/>
+        <item x="611"/>
+        <item x="612"/>
+        <item x="613"/>
+        <item x="614"/>
+        <item x="615"/>
+        <item x="616"/>
+        <item x="617"/>
+        <item x="618"/>
+        <item x="619"/>
+        <item x="620"/>
+        <item x="621"/>
+        <item x="622"/>
+        <item x="623"/>
+        <item x="624"/>
+        <item x="625"/>
+        <item x="626"/>
+        <item x="627"/>
+        <item x="628"/>
+        <item x="629"/>
+        <item x="630"/>
+        <item x="631"/>
+        <item x="632"/>
+        <item x="633"/>
+        <item x="634"/>
+        <item x="635"/>
+        <item x="636"/>
+        <item x="637"/>
+        <item x="638"/>
+        <item x="639"/>
+        <item x="640"/>
+        <item x="641"/>
+        <item x="642"/>
+        <item x="643"/>
+        <item x="644"/>
+        <item x="645"/>
+        <item x="646"/>
+        <item x="647"/>
+        <item x="648"/>
+        <item x="649"/>
+        <item x="650"/>
+        <item x="651"/>
+        <item x="652"/>
+        <item x="653"/>
+        <item x="654"/>
+        <item x="655"/>
+        <item x="656"/>
+        <item x="657"/>
+        <item x="658"/>
+        <item x="659"/>
+        <item x="660"/>
+        <item x="661"/>
+        <item x="662"/>
+        <item x="663"/>
+        <item x="664"/>
+        <item x="665"/>
+        <item x="666"/>
+        <item x="667"/>
+        <item x="668"/>
+        <item x="669"/>
+        <item x="670"/>
+        <item x="671"/>
+        <item x="672"/>
+        <item x="673"/>
+        <item x="674"/>
+        <item x="675"/>
+        <item x="676"/>
+        <item x="677"/>
+        <item x="678"/>
+        <item x="679"/>
+        <item x="680"/>
+        <item x="681"/>
+        <item x="682"/>
+        <item x="683"/>
+        <item x="684"/>
+        <item x="685"/>
+        <item x="686"/>
+        <item x="687"/>
+        <item x="688"/>
+        <item x="689"/>
+        <item x="690"/>
+        <item x="691"/>
+        <item x="692"/>
+        <item x="693"/>
+        <item x="694"/>
+        <item x="695"/>
+        <item x="696"/>
+        <item x="697"/>
+        <item x="698"/>
+        <item x="699"/>
+        <item x="700"/>
+        <item x="701"/>
+        <item x="702"/>
+        <item x="703"/>
+        <item x="704"/>
+        <item x="705"/>
+        <item x="706"/>
+        <item x="707"/>
+        <item x="708"/>
+        <item x="709"/>
+        <item x="710"/>
+        <item x="711"/>
+        <item x="712"/>
+        <item x="713"/>
+        <item x="714"/>
+        <item x="715"/>
+        <item x="716"/>
+        <item x="717"/>
+        <item x="718"/>
+        <item x="719"/>
+        <item x="720"/>
+        <item x="721"/>
+        <item x="722"/>
+        <item x="723"/>
+        <item x="724"/>
+        <item x="725"/>
+        <item x="726"/>
+        <item x="727"/>
+        <item x="728"/>
+        <item x="729"/>
+        <item x="730"/>
+        <item x="731"/>
+        <item x="732"/>
+        <item x="733"/>
+        <item x="734"/>
+        <item x="735"/>
+        <item x="736"/>
+        <item x="737"/>
+        <item x="738"/>
+        <item x="739"/>
+        <item x="740"/>
+        <item x="741"/>
+        <item x="742"/>
+        <item x="743"/>
+        <item x="744"/>
+        <item x="745"/>
+        <item x="746"/>
+        <item x="747"/>
+        <item x="748"/>
+        <item x="749"/>
+        <item x="750"/>
+        <item x="751"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of identifier " fld="0" subtotal="count" baseField="1" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{312C896D-2568-4831-929B-78CBF05CBF07}" name="PivotTable10" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A2:A3" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="3">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of identifier " fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0FAB2BC0-9373-4DBB-9431-E13A8ACAB598}" name="TableA" displayName="TableA" ref="A1:C1002" totalsRowShown="0">
   <autoFilter ref="A1:C1002" xr:uid="{0FAB2BC0-9373-4DBB-9431-E13A8ACAB598}"/>
@@ -16983,10 +19624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40885E39-B325-4D8A-BE5B-FC3BDDAD67B0}">
-  <dimension ref="A1:C1002"/>
+  <dimension ref="A1:D1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1002" sqref="A1:C1002"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16996,7 +19637,7 @@
     <col min="3" max="3" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17007,7 +19648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -17017,8 +19658,12 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>MIN(A:A)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1001</v>
       </c>
@@ -17028,8 +19673,12 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f>MAX(A:A)</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1002</v>
       </c>
@@ -17040,7 +19689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1003</v>
       </c>
@@ -17051,7 +19700,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1004</v>
       </c>
@@ -17062,7 +19711,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1005</v>
       </c>
@@ -17073,7 +19722,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1006</v>
       </c>
@@ -17084,7 +19733,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1007</v>
       </c>
@@ -17095,7 +19744,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1008</v>
       </c>
@@ -17106,7 +19755,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1009</v>
       </c>
@@ -17117,7 +19766,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1010</v>
       </c>
@@ -17128,7 +19777,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1011</v>
       </c>
@@ -17139,7 +19788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1012</v>
       </c>
@@ -17150,7 +19799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1013</v>
       </c>
@@ -17161,7 +19810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1014</v>
       </c>
@@ -28028,10 +30677,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E45F09-0A17-4605-A09B-7413CA0C6FD3}">
-  <dimension ref="A1:B753"/>
+  <dimension ref="A1:C753"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28040,7 +30689,7 @@
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -28048,23 +30697,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1457</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <f>MIN(A:A)</f>
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1458</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <f>MAX(A:A)</f>
+        <v>2381</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1461</v>
       </c>
@@ -28072,7 +30729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1463</v>
       </c>
@@ -28080,7 +30737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1465</v>
       </c>
@@ -28088,7 +30745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1468</v>
       </c>
@@ -28096,7 +30753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1470</v>
       </c>
@@ -28104,7 +30761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1471</v>
       </c>
@@ -28112,7 +30769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1562</v>
       </c>
@@ -28120,7 +30777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1563</v>
       </c>
@@ -28128,7 +30785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1569</v>
       </c>
@@ -28136,7 +30793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1576</v>
       </c>
@@ -28144,7 +30801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1577</v>
       </c>
@@ -28152,7 +30809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1578</v>
       </c>
@@ -28160,7 +30817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1579</v>
       </c>
@@ -49127,410 +51784,482 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC92C0C-DB47-4A1F-BFC3-FD5B3AF8ACB0}">
-  <dimension ref="A2:K23"/>
+  <dimension ref="A2:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:E17"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1001</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3">
         <v>508</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
       <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3">
+      <c r="D4" s="3">
         <v>2</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="I4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="3">
         <v>261</v>
       </c>
-      <c r="I4" s="3">
+      <c r="K4" s="3">
         <v>247</v>
       </c>
-      <c r="J4" s="3">
+      <c r="L4" s="3">
         <v>508</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3">
         <v>491</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="3">
-        <v>2</v>
-      </c>
-      <c r="I5" s="3"/>
       <c r="J5" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="K5" s="3"/>
+      <c r="L5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="D6" s="3">
         <v>1001</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="I6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="3">
         <v>251</v>
       </c>
-      <c r="I6" s="3">
+      <c r="K6" s="3">
         <v>240</v>
       </c>
-      <c r="J6" s="3">
+      <c r="L6" s="3">
         <v>491</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G7" s="2" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="3">
+      <c r="J7" s="3">
         <v>514</v>
       </c>
-      <c r="I7" s="3">
+      <c r="K7" s="3">
         <v>487</v>
       </c>
-      <c r="J7" s="3">
+      <c r="L7" s="3">
         <v>1001</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>2000</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>752</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>748</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B11">
+      <c r="D12">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12">
+      <c r="D13">
         <v>752</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>1457</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>2381</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>1001</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
         <v>12</v>
       </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19" t="s">
         <v>2</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L19" t="s">
         <v>14</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>1</v>
-      </c>
-      <c r="B16">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20">
         <v>156</v>
       </c>
-      <c r="C16">
+      <c r="E20">
         <v>2</v>
       </c>
-      <c r="D16">
+      <c r="F20">
         <v>209</v>
       </c>
-      <c r="E16">
+      <c r="G20">
         <v>367</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="3">
+      <c r="I20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="3">
         <v>185</v>
       </c>
-      <c r="I16" s="3">
+      <c r="K20" s="3">
         <v>4</v>
       </c>
-      <c r="J16" s="3">
+      <c r="L20" s="3">
         <v>325</v>
       </c>
-      <c r="K16" s="3">
+      <c r="M20" s="3">
         <v>514</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B17">
+      <c r="D21">
         <v>2</v>
       </c>
-      <c r="D17">
+      <c r="F21">
         <v>2</v>
       </c>
-      <c r="E17">
+      <c r="G21">
         <v>4</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="3">
+      <c r="I21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="3">
         <v>92</v>
       </c>
-      <c r="I17" s="3">
+      <c r="K21" s="3">
         <v>2</v>
       </c>
-      <c r="J17" s="3">
+      <c r="L21" s="3">
         <v>167</v>
       </c>
-      <c r="K17" s="3">
+      <c r="M21" s="3">
         <v>261</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18">
+      <c r="D22">
         <v>350</v>
       </c>
-      <c r="D18">
+      <c r="F22">
         <v>280</v>
       </c>
-      <c r="E18">
+      <c r="G22">
         <v>630</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="I22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="3">
+      <c r="J22" s="3">
         <v>2</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3">
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B19">
+      <c r="D23">
         <v>508</v>
       </c>
-      <c r="C19">
+      <c r="E23">
         <v>2</v>
       </c>
-      <c r="D19">
+      <c r="F23">
         <v>491</v>
       </c>
-      <c r="E19">
+      <c r="G23">
         <v>1001</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="3">
+      <c r="I23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="3">
         <v>91</v>
       </c>
-      <c r="I19" s="3">
+      <c r="K23" s="3">
         <v>2</v>
       </c>
-      <c r="J19" s="3">
+      <c r="L23" s="3">
         <v>158</v>
       </c>
-      <c r="K19" s="3">
+      <c r="M23" s="3">
         <v>251</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>2000</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="3">
         <v>182</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3">
+      <c r="K24" s="3"/>
+      <c r="L24" s="3">
         <v>305</v>
       </c>
-      <c r="K20" s="3">
+      <c r="M24" s="3">
         <v>487</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" s="3">
         <v>64</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3">
+      <c r="K25" s="3"/>
+      <c r="L25" s="3">
         <v>183</v>
       </c>
-      <c r="K21" s="3">
+      <c r="M25" s="3">
         <v>247</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="3">
         <v>118</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3">
+      <c r="K26" s="3"/>
+      <c r="L26" s="3">
         <v>122</v>
       </c>
-      <c r="K22" s="3">
+      <c r="M26" s="3">
         <v>240</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G23" s="2" t="s">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I27" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H23" s="3">
+      <c r="J27" s="3">
         <v>367</v>
       </c>
-      <c r="I23" s="3">
+      <c r="K27" s="3">
         <v>4</v>
       </c>
-      <c r="J23" s="3">
+      <c r="L27" s="3">
         <v>630</v>
       </c>
-      <c r="K23" s="3">
+      <c r="M27" s="3">
         <v>1001</v>
       </c>
     </row>

</xml_diff>